<commit_message>
added the sql queries
</commit_message>
<xml_diff>
--- a/CaseStudyDatabaseStructure.xlsx
+++ b/CaseStudyDatabaseStructure.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="139">
   <si>
     <t>First_Name</t>
   </si>
@@ -1315,6 +1315,23 @@
         <scheme val="minor"/>
       </rPr>
       <t>VARCHAR(15)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O_ID(FK) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INT</t>
     </r>
   </si>
 </sst>
@@ -1996,8 +2013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2303,6 +2320,9 @@
       <c r="C25" t="s">
         <v>127</v>
       </c>
+      <c r="D25" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">

</xml_diff>

<commit_message>
can now fully insert a meal along with payments
</commit_message>
<xml_diff>
--- a/CaseStudyDatabaseStructure.xlsx
+++ b/CaseStudyDatabaseStructure.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
   <si>
     <t>First_Name</t>
   </si>
@@ -1336,13 +1336,19 @@
   </si>
   <si>
     <t>price double</t>
+  </si>
+  <si>
+    <t>delivery_time</t>
+  </si>
+  <si>
+    <t>Credit_Card_Details (CHANGE NAME)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1390,6 +1396,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1411,10 +1424,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2024,8 +2038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,7 +2047,7 @@
     <col min="1" max="1" width="29.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="31.140625" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
@@ -2170,6 +2184,9 @@
       <c r="D10" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="F10" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2287,7 +2304,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>72</v>

</xml_diff>